<commit_message>
added 1 more node for monitoring to aws planning spreadsheet
</commit_message>
<xml_diff>
--- a/wiki/aws-planning/aws-infra-planning.xlsx
+++ b/wiki/aws-planning/aws-infra-planning.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18431"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18528"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="268" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="91">
   <si>
     <t>Public</t>
   </si>
@@ -297,6 +297,9 @@
   </si>
   <si>
     <t>Total Cost</t>
+  </si>
+  <si>
+    <t>infra-monitoring</t>
   </si>
 </sst>
 </file>
@@ -876,10 +879,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M56"/>
+  <dimension ref="A1:M57"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4:J4"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1167,136 +1170,139 @@
       <c r="C10" s="7">
         <v>1</v>
       </c>
-      <c r="D10" t="s">
-        <v>67</v>
-      </c>
-      <c r="E10" t="s">
-        <v>67</v>
+      <c r="D10" s="7" t="s">
+        <v>90</v>
+      </c>
+      <c r="E10" s="7" t="s">
+        <v>90</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="G10" s="7">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H10" s="7">
         <v>1</v>
       </c>
       <c r="J10" s="6">
-        <v>1.1599999999999999E-2</v>
+        <v>4.6399999999999997E-2</v>
       </c>
       <c r="K10" s="9">
         <f t="shared" ref="K10" si="6">J10*780</f>
-        <v>9.048</v>
+        <v>36.192</v>
       </c>
       <c r="L10" s="9">
         <f t="shared" ref="L10" si="7">K10*12</f>
+        <v>434.30399999999997</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="C11" s="7">
+        <v>1</v>
+      </c>
+      <c r="D11" t="s">
+        <v>67</v>
+      </c>
+      <c r="E11" t="s">
+        <v>67</v>
+      </c>
+      <c r="F11" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="G11" s="7">
+        <v>1</v>
+      </c>
+      <c r="H11" s="7">
+        <v>1</v>
+      </c>
+      <c r="J11" s="6">
+        <v>1.1599999999999999E-2</v>
+      </c>
+      <c r="K11" s="9">
+        <f t="shared" ref="K11" si="8">J11*780</f>
+        <v>9.048</v>
+      </c>
+      <c r="L11" s="9">
+        <f t="shared" ref="L11" si="9">K11*12</f>
         <v>108.57599999999999</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="F11" s="4"/>
-      <c r="J11" s="6"/>
-    </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="C12" s="1">
-        <f>SUM(C3:C10)</f>
-        <v>8</v>
-      </c>
-      <c r="D12" s="1"/>
-      <c r="F12" s="1"/>
-      <c r="G12" s="1"/>
-      <c r="H12" s="1"/>
-      <c r="I12" s="1"/>
-      <c r="J12" s="3">
+      <c r="F12" s="4"/>
+      <c r="J12" s="6"/>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="C13" s="1">
+        <f>SUM(C3:C11)</f>
+        <v>9</v>
+      </c>
+      <c r="D13" s="1"/>
+      <c r="F13" s="1"/>
+      <c r="G13" s="1"/>
+      <c r="H13" s="1"/>
+      <c r="I13" s="1"/>
+      <c r="J13" s="3">
         <f>SUM(J3:J9)</f>
         <v>0.18559999999999999</v>
       </c>
-      <c r="K12" s="2">
-        <f>SUM(K3:K10)</f>
-        <v>153.816</v>
-      </c>
-      <c r="L12" s="2">
+      <c r="K13" s="2">
+        <f>SUM(K3:K11)</f>
+        <v>190.00800000000001</v>
+      </c>
+      <c r="L13" s="2">
         <f>SUM(L3:L9)</f>
         <v>1737.2159999999999</v>
       </c>
     </row>
-    <row r="14" spans="1:13" ht="18" x14ac:dyDescent="0.35">
-      <c r="A14" s="5" t="s">
+    <row r="15" spans="1:13" ht="18" x14ac:dyDescent="0.35">
+      <c r="A15" s="5" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="B15" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C15" s="1" t="s">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="B16" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C16" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D15" s="1" t="s">
+      <c r="D16" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E15" s="1"/>
-      <c r="F15" s="1" t="s">
+      <c r="E16" s="1"/>
+      <c r="F16" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="G15" s="1" t="s">
+      <c r="G16" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="H15" s="1" t="s">
+      <c r="H16" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="I15" s="1" t="s">
+      <c r="I16" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="J15" s="3" t="s">
+      <c r="J16" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="K15" s="2" t="s">
+      <c r="K16" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="L15" s="2" t="s">
+      <c r="L16" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="M15" s="1"/>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="B16" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="C16" s="7">
-        <v>1</v>
-      </c>
-      <c r="D16" s="7" t="s">
+      <c r="M16" s="1"/>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="B17" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="C17" s="7">
+        <v>1</v>
+      </c>
+      <c r="D17" s="7" t="s">
         <v>11</v>
-      </c>
-      <c r="F16" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="G16" s="7">
-        <v>1</v>
-      </c>
-      <c r="H16" s="7">
-        <v>1</v>
-      </c>
-      <c r="J16" s="6">
-        <v>1.6E-2</v>
-      </c>
-      <c r="K16" s="9">
-        <f>J16*780</f>
-        <v>12.48</v>
-      </c>
-      <c r="L16" s="9">
-        <f>K16*12</f>
-        <v>149.76</v>
-      </c>
-    </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="C17" s="7">
-        <v>1</v>
-      </c>
-      <c r="D17" s="7" t="s">
-        <v>13</v>
       </c>
       <c r="F17" s="4" t="s">
         <v>17</v>
@@ -1311,23 +1317,20 @@
         <v>1.6E-2</v>
       </c>
       <c r="K17" s="9">
-        <f t="shared" ref="K17:K21" si="8">J17*780</f>
+        <f>J17*780</f>
         <v>12.48</v>
       </c>
       <c r="L17" s="9">
-        <f t="shared" ref="L17:L21" si="9">K17*12</f>
+        <f>K17*12</f>
         <v>149.76</v>
       </c>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="B18" s="7" t="s">
-        <v>14</v>
-      </c>
       <c r="C18" s="7">
         <v>1</v>
       </c>
       <c r="D18" s="7" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F18" s="4" t="s">
         <v>17</v>
@@ -1342,20 +1345,23 @@
         <v>1.6E-2</v>
       </c>
       <c r="K18" s="9">
-        <f t="shared" si="8"/>
+        <f t="shared" ref="K18:K22" si="10">J18*780</f>
         <v>12.48</v>
       </c>
       <c r="L18" s="9">
-        <f t="shared" si="9"/>
+        <f t="shared" ref="L18:L22" si="11">K18*12</f>
         <v>149.76</v>
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="B19" s="7" t="s">
+        <v>14</v>
+      </c>
       <c r="C19" s="7">
         <v>1</v>
       </c>
       <c r="D19" s="7" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="F19" s="4" t="s">
         <v>17</v>
@@ -1370,11 +1376,11 @@
         <v>1.6E-2</v>
       </c>
       <c r="K19" s="9">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>12.48</v>
       </c>
       <c r="L19" s="9">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>149.76</v>
       </c>
     </row>
@@ -1383,13 +1389,13 @@
         <v>1</v>
       </c>
       <c r="D20" s="7" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="F20" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G20" s="7">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="H20" s="7">
         <v>1</v>
@@ -1398,11 +1404,11 @@
         <v>1.6E-2</v>
       </c>
       <c r="K20" s="9">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>12.48</v>
       </c>
       <c r="L20" s="9">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>149.76</v>
       </c>
     </row>
@@ -1411,7 +1417,7 @@
         <v>1</v>
       </c>
       <c r="D21" s="7" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="F21" s="4" t="s">
         <v>18</v>
@@ -1426,113 +1432,113 @@
         <v>1.6E-2</v>
       </c>
       <c r="K21" s="9">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>12.48</v>
       </c>
       <c r="L21" s="9">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>149.76</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="C23" s="1">
-        <f>SUM(C16:C22)</f>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="C22" s="7">
+        <v>1</v>
+      </c>
+      <c r="D22" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="F22" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="G22" s="7">
+        <v>4</v>
+      </c>
+      <c r="H22" s="7">
+        <v>1</v>
+      </c>
+      <c r="J22" s="6">
+        <v>1.6E-2</v>
+      </c>
+      <c r="K22" s="9">
+        <f t="shared" si="10"/>
+        <v>12.48</v>
+      </c>
+      <c r="L22" s="9">
+        <f t="shared" si="11"/>
+        <v>149.76</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="C24" s="1">
+        <f>SUM(C17:C23)</f>
         <v>6</v>
       </c>
-      <c r="D23" s="1"/>
-      <c r="F23" s="1"/>
-      <c r="G23" s="1"/>
-      <c r="H23" s="1"/>
-      <c r="I23" s="1"/>
-      <c r="J23" s="3">
-        <f>SUM(J16:J22)</f>
+      <c r="D24" s="1"/>
+      <c r="F24" s="1"/>
+      <c r="G24" s="1"/>
+      <c r="H24" s="1"/>
+      <c r="I24" s="1"/>
+      <c r="J24" s="3">
+        <f>SUM(J17:J23)</f>
         <v>9.6000000000000002E-2</v>
       </c>
-      <c r="K23" s="2">
-        <f>SUM(K16:K22)</f>
+      <c r="K24" s="2">
+        <f>SUM(K17:K23)</f>
         <v>74.88000000000001</v>
       </c>
-      <c r="L23" s="2">
-        <f>SUM(L16:L22)</f>
+      <c r="L24" s="2">
+        <f>SUM(L17:L23)</f>
         <v>898.56</v>
       </c>
     </row>
-    <row r="25" spans="1:13" ht="18" x14ac:dyDescent="0.35">
-      <c r="A25" s="5" t="s">
+    <row r="26" spans="1:13" ht="18" x14ac:dyDescent="0.35">
+      <c r="A26" s="5" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="B26" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C26" s="1" t="s">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="B27" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C27" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D26" s="1" t="s">
+      <c r="D27" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E26" s="1"/>
-      <c r="F26" s="1" t="s">
+      <c r="E27" s="1"/>
+      <c r="F27" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="G26" s="1" t="s">
+      <c r="G27" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="H26" s="1" t="s">
+      <c r="H27" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="I26" s="1" t="s">
+      <c r="I27" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="J26" s="3" t="s">
+      <c r="J27" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="K26" s="2" t="s">
+      <c r="K27" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="L26" s="2" t="s">
+      <c r="L27" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="M26" s="1"/>
-    </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="B27" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="C27" s="7">
-        <v>1</v>
-      </c>
-      <c r="D27" s="7" t="s">
+      <c r="M27" s="1"/>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="B28" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="C28" s="7">
+        <v>1</v>
+      </c>
+      <c r="D28" s="7" t="s">
         <v>11</v>
-      </c>
-      <c r="F27" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="G27" s="7">
-        <v>1</v>
-      </c>
-      <c r="H27" s="7">
-        <v>1</v>
-      </c>
-      <c r="J27" s="6">
-        <v>6.0000000000000001E-3</v>
-      </c>
-      <c r="K27" s="9">
-        <f>J27*780</f>
-        <v>4.68</v>
-      </c>
-      <c r="L27" s="9">
-        <f>K27*12</f>
-        <v>56.16</v>
-      </c>
-    </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="C28" s="7">
-        <v>1</v>
-      </c>
-      <c r="D28" s="7" t="s">
-        <v>13</v>
       </c>
       <c r="F28" s="4" t="s">
         <v>17</v>
@@ -1547,23 +1553,20 @@
         <v>6.0000000000000001E-3</v>
       </c>
       <c r="K28" s="9">
-        <f t="shared" ref="K28:K32" si="10">J28*780</f>
+        <f>J28*780</f>
         <v>4.68</v>
       </c>
       <c r="L28" s="9">
-        <f t="shared" ref="L28:L32" si="11">K28*12</f>
+        <f>K28*12</f>
         <v>56.16</v>
       </c>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="B29" s="7" t="s">
-        <v>14</v>
-      </c>
       <c r="C29" s="7">
         <v>1</v>
       </c>
       <c r="D29" s="7" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F29" s="4" t="s">
         <v>17</v>
@@ -1578,20 +1581,23 @@
         <v>6.0000000000000001E-3</v>
       </c>
       <c r="K29" s="9">
-        <f t="shared" si="10"/>
+        <f t="shared" ref="K29:K33" si="12">J29*780</f>
         <v>4.68</v>
       </c>
       <c r="L29" s="9">
-        <f t="shared" si="11"/>
+        <f t="shared" ref="L29:L33" si="13">K29*12</f>
         <v>56.16</v>
       </c>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="B30" s="7" t="s">
+        <v>14</v>
+      </c>
       <c r="C30" s="7">
         <v>1</v>
       </c>
       <c r="D30" s="7" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="F30" s="4" t="s">
         <v>17</v>
@@ -1606,11 +1612,11 @@
         <v>6.0000000000000001E-3</v>
       </c>
       <c r="K30" s="9">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>4.68</v>
       </c>
       <c r="L30" s="9">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>56.16</v>
       </c>
     </row>
@@ -1619,27 +1625,27 @@
         <v>1</v>
       </c>
       <c r="D31" s="7" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="F31" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G31" s="7">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="H31" s="7">
         <v>1</v>
       </c>
       <c r="J31" s="6">
-        <v>2.4E-2</v>
+        <v>6.0000000000000001E-3</v>
       </c>
       <c r="K31" s="9">
-        <f t="shared" si="10"/>
-        <v>18.72</v>
+        <f t="shared" si="12"/>
+        <v>4.68</v>
       </c>
       <c r="L31" s="9">
-        <f t="shared" si="11"/>
-        <v>224.64</v>
+        <f t="shared" si="13"/>
+        <v>56.16</v>
       </c>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.3">
@@ -1647,7 +1653,7 @@
         <v>1</v>
       </c>
       <c r="D32" s="7" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="F32" s="4" t="s">
         <v>18</v>
@@ -1662,124 +1668,124 @@
         <v>2.4E-2</v>
       </c>
       <c r="K32" s="9">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>18.72</v>
       </c>
       <c r="L32" s="9">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>224.64</v>
       </c>
     </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="C34" s="1">
-        <f>SUM(C27:C33)</f>
+    <row r="33" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="C33" s="7">
+        <v>1</v>
+      </c>
+      <c r="D33" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="F33" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="G33" s="7">
+        <v>4</v>
+      </c>
+      <c r="H33" s="7">
+        <v>1</v>
+      </c>
+      <c r="J33" s="6">
+        <v>2.4E-2</v>
+      </c>
+      <c r="K33" s="9">
+        <f t="shared" si="12"/>
+        <v>18.72</v>
+      </c>
+      <c r="L33" s="9">
+        <f t="shared" si="13"/>
+        <v>224.64</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="C35" s="1">
+        <f>SUM(C28:C34)</f>
         <v>6</v>
       </c>
-      <c r="D34" s="1"/>
-      <c r="F34" s="1"/>
-      <c r="G34" s="1"/>
-      <c r="H34" s="1"/>
-      <c r="I34" s="1"/>
-      <c r="J34" s="3">
-        <f>SUM(J27:J33)</f>
-        <v>7.2000000000000008E-2</v>
-      </c>
-      <c r="K34" s="2">
-        <f>SUM(K27:K33)</f>
-        <v>56.16</v>
-      </c>
-      <c r="L34" s="2">
-        <f>SUM(L27:L33)</f>
-        <v>673.92</v>
-      </c>
-    </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="C35" s="1"/>
       <c r="D35" s="1"/>
       <c r="F35" s="1"/>
       <c r="G35" s="1"/>
       <c r="H35" s="1"/>
       <c r="I35" s="1"/>
-      <c r="J35" s="3"/>
-      <c r="K35" s="2"/>
-      <c r="L35" s="2"/>
-    </row>
-    <row r="36" spans="1:13" ht="18" x14ac:dyDescent="0.35">
-      <c r="A36" s="5" t="s">
+      <c r="J35" s="3">
+        <f>SUM(J28:J34)</f>
+        <v>7.2000000000000008E-2</v>
+      </c>
+      <c r="K35" s="2">
+        <f>SUM(K28:K34)</f>
+        <v>56.16</v>
+      </c>
+      <c r="L35" s="2">
+        <f>SUM(L28:L34)</f>
+        <v>673.92</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="C36" s="1"/>
+      <c r="D36" s="1"/>
+      <c r="F36" s="1"/>
+      <c r="G36" s="1"/>
+      <c r="H36" s="1"/>
+      <c r="I36" s="1"/>
+      <c r="J36" s="3"/>
+      <c r="K36" s="2"/>
+      <c r="L36" s="2"/>
+    </row>
+    <row r="37" spans="1:13" ht="18" x14ac:dyDescent="0.35">
+      <c r="A37" s="5" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="B37" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C37" s="1" t="s">
+    <row r="38" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="B38" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C38" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D37" s="1" t="s">
+      <c r="D38" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E37" s="1"/>
-      <c r="F37" s="1" t="s">
+      <c r="E38" s="1"/>
+      <c r="F38" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="G37" s="1" t="s">
+      <c r="G38" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="H37" s="1" t="s">
+      <c r="H38" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="I37" s="1" t="s">
+      <c r="I38" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="J37" s="3" t="s">
+      <c r="J38" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="K37" s="2" t="s">
+      <c r="K38" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="L37" s="2" t="s">
+      <c r="L38" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="M37" s="1"/>
-    </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="B38" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="C38" s="7">
-        <v>1</v>
-      </c>
-      <c r="D38" s="7" t="s">
+      <c r="M38" s="1"/>
+    </row>
+    <row r="39" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="B39" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="C39" s="7">
+        <v>1</v>
+      </c>
+      <c r="D39" s="7" t="s">
         <v>11</v>
-      </c>
-      <c r="F38" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="G38" s="7">
-        <v>1</v>
-      </c>
-      <c r="H38" s="7">
-        <v>1</v>
-      </c>
-      <c r="J38" s="6">
-        <f>K38/780</f>
-        <v>7.3717948717948716E-3</v>
-      </c>
-      <c r="K38" s="9">
-        <f>L38/12</f>
-        <v>5.75</v>
-      </c>
-      <c r="L38" s="9">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="C39" s="7">
-        <v>1</v>
-      </c>
-      <c r="D39" s="7" t="s">
-        <v>13</v>
       </c>
       <c r="F39" s="4" t="s">
         <v>17</v>
@@ -1791,11 +1797,11 @@
         <v>1</v>
       </c>
       <c r="J39" s="6">
-        <f t="shared" ref="J39:J43" si="12">K39/780</f>
+        <f>K39/780</f>
         <v>7.3717948717948716E-3</v>
       </c>
       <c r="K39" s="9">
-        <f t="shared" ref="K39:K43" si="13">L39/12</f>
+        <f>L39/12</f>
         <v>5.75</v>
       </c>
       <c r="L39" s="9">
@@ -1803,14 +1809,11 @@
       </c>
     </row>
     <row r="40" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="B40" s="7" t="s">
-        <v>14</v>
-      </c>
       <c r="C40" s="7">
         <v>1</v>
       </c>
       <c r="D40" s="7" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F40" s="4" t="s">
         <v>17</v>
@@ -1822,11 +1825,11 @@
         <v>1</v>
       </c>
       <c r="J40" s="6">
-        <f t="shared" si="12"/>
+        <f t="shared" ref="J40:J44" si="14">K40/780</f>
         <v>7.3717948717948716E-3</v>
       </c>
       <c r="K40" s="9">
-        <f t="shared" si="13"/>
+        <f t="shared" ref="K40:K44" si="15">L40/12</f>
         <v>5.75</v>
       </c>
       <c r="L40" s="9">
@@ -1834,11 +1837,14 @@
       </c>
     </row>
     <row r="41" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="B41" s="7" t="s">
+        <v>14</v>
+      </c>
       <c r="C41" s="7">
         <v>1</v>
       </c>
       <c r="D41" s="7" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="F41" s="4" t="s">
         <v>17</v>
@@ -1850,11 +1856,11 @@
         <v>1</v>
       </c>
       <c r="J41" s="6">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>7.3717948717948716E-3</v>
       </c>
       <c r="K41" s="9">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>5.75</v>
       </c>
       <c r="L41" s="9">
@@ -1866,27 +1872,27 @@
         <v>1</v>
       </c>
       <c r="D42" s="7" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="F42" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G42" s="7">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="H42" s="7">
         <v>1</v>
       </c>
       <c r="J42" s="6">
-        <f t="shared" si="12"/>
-        <v>2.9380341880341884E-2</v>
+        <f t="shared" si="14"/>
+        <v>7.3717948717948716E-3</v>
       </c>
       <c r="K42" s="9">
-        <f t="shared" si="13"/>
-        <v>22.916666666666668</v>
+        <f t="shared" si="15"/>
+        <v>5.75</v>
       </c>
       <c r="L42" s="9">
-        <v>275</v>
+        <v>69</v>
       </c>
     </row>
     <row r="43" spans="1:13" x14ac:dyDescent="0.3">
@@ -1894,7 +1900,7 @@
         <v>1</v>
       </c>
       <c r="D43" s="7" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="F43" s="4" t="s">
         <v>18</v>
@@ -1906,116 +1912,116 @@
         <v>1</v>
       </c>
       <c r="J43" s="6">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>2.9380341880341884E-2</v>
       </c>
       <c r="K43" s="9">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>22.916666666666668</v>
       </c>
       <c r="L43" s="9">
         <v>275</v>
       </c>
     </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="C45" s="1">
-        <f>SUM(C38:C44)</f>
+    <row r="44" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="C44" s="7">
+        <v>1</v>
+      </c>
+      <c r="D44" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="F44" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="G44" s="7">
+        <v>4</v>
+      </c>
+      <c r="H44" s="7">
+        <v>1</v>
+      </c>
+      <c r="J44" s="6">
+        <f t="shared" si="14"/>
+        <v>2.9380341880341884E-2</v>
+      </c>
+      <c r="K44" s="9">
+        <f t="shared" si="15"/>
+        <v>22.916666666666668</v>
+      </c>
+      <c r="L44" s="9">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="46" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="C46" s="1">
+        <f>SUM(C39:C45)</f>
         <v>6</v>
       </c>
-      <c r="D45" s="1"/>
-      <c r="F45" s="1"/>
-      <c r="G45" s="1"/>
-      <c r="H45" s="1"/>
-      <c r="I45" s="1"/>
-      <c r="J45" s="3">
-        <f>SUM(J38:J44)</f>
+      <c r="D46" s="1"/>
+      <c r="F46" s="1"/>
+      <c r="G46" s="1"/>
+      <c r="H46" s="1"/>
+      <c r="I46" s="1"/>
+      <c r="J46" s="3">
+        <f>SUM(J39:J45)</f>
         <v>8.8247863247863254E-2</v>
       </c>
-      <c r="K45" s="2">
-        <f>SUM(K38:K44)</f>
+      <c r="K46" s="2">
+        <f>SUM(K39:K45)</f>
         <v>68.833333333333343</v>
       </c>
-      <c r="L45" s="2">
-        <f>SUM(L38:L44)</f>
+      <c r="L46" s="2">
+        <f>SUM(L39:L45)</f>
         <v>826</v>
       </c>
     </row>
-    <row r="47" spans="1:13" ht="18" x14ac:dyDescent="0.35">
-      <c r="A47" s="5" t="s">
+    <row r="48" spans="1:13" ht="18" x14ac:dyDescent="0.35">
+      <c r="A48" s="5" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="48" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="B48" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C48" s="1" t="s">
+    <row r="49" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B49" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C49" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D48" s="1" t="s">
+      <c r="D49" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E48" s="1"/>
-      <c r="F48" s="1" t="s">
+      <c r="E49" s="1"/>
+      <c r="F49" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="G48" s="1" t="s">
+      <c r="G49" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="H48" s="1" t="s">
+      <c r="H49" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="I48" s="1" t="s">
+      <c r="I49" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="J48" s="3" t="s">
+      <c r="J49" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="K48" s="2" t="s">
+      <c r="K49" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="L48" s="2" t="s">
+      <c r="L49" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="M48" s="1"/>
-    </row>
-    <row r="49" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B49" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="C49" s="7">
-        <v>1</v>
-      </c>
-      <c r="D49" s="7" t="s">
+      <c r="M49" s="1"/>
+    </row>
+    <row r="50" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B50" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="C50" s="7">
+        <v>1</v>
+      </c>
+      <c r="D50" s="7" t="s">
         <v>11</v>
-      </c>
-      <c r="F49" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="G49" s="7">
-        <v>1</v>
-      </c>
-      <c r="H49" s="7">
-        <v>1</v>
-      </c>
-      <c r="J49" s="6">
-        <f>K49/780</f>
-        <v>1.3247863247863249E-2</v>
-      </c>
-      <c r="K49" s="9">
-        <f>L49/12</f>
-        <v>10.333333333333334</v>
-      </c>
-      <c r="L49" s="9">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="50" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="C50" s="7">
-        <v>1</v>
-      </c>
-      <c r="D50" s="7" t="s">
-        <v>13</v>
       </c>
       <c r="F50" s="4" t="s">
         <v>17</v>
@@ -2027,26 +2033,23 @@
         <v>1</v>
       </c>
       <c r="J50" s="6">
-        <f t="shared" ref="J50:J54" si="14">K50/780</f>
+        <f>K50/780</f>
         <v>1.3247863247863249E-2</v>
       </c>
       <c r="K50" s="9">
-        <f t="shared" ref="K50:K54" si="15">L50/12</f>
+        <f>L50/12</f>
         <v>10.333333333333334</v>
       </c>
       <c r="L50" s="9">
         <v>124</v>
       </c>
     </row>
-    <row r="51" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B51" s="7" t="s">
-        <v>14</v>
-      </c>
+    <row r="51" spans="2:13" x14ac:dyDescent="0.3">
       <c r="C51" s="7">
         <v>1</v>
       </c>
       <c r="D51" s="7" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F51" s="4" t="s">
         <v>17</v>
@@ -2058,23 +2061,26 @@
         <v>1</v>
       </c>
       <c r="J51" s="6">
-        <f t="shared" si="14"/>
+        <f t="shared" ref="J51:J55" si="16">K51/780</f>
         <v>1.3247863247863249E-2</v>
       </c>
       <c r="K51" s="9">
-        <f t="shared" si="15"/>
+        <f t="shared" ref="K51:K55" si="17">L51/12</f>
         <v>10.333333333333334</v>
       </c>
       <c r="L51" s="9">
         <v>124</v>
       </c>
     </row>
-    <row r="52" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="52" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B52" s="7" t="s">
+        <v>14</v>
+      </c>
       <c r="C52" s="7">
         <v>1</v>
       </c>
       <c r="D52" s="7" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="F52" s="4" t="s">
         <v>17</v>
@@ -2086,51 +2092,51 @@
         <v>1</v>
       </c>
       <c r="J52" s="6">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>1.3247863247863249E-2</v>
       </c>
       <c r="K52" s="9">
-        <f t="shared" si="15"/>
+        <f t="shared" si="17"/>
         <v>10.333333333333334</v>
       </c>
       <c r="L52" s="9">
         <v>124</v>
       </c>
     </row>
-    <row r="53" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="53" spans="2:13" x14ac:dyDescent="0.3">
       <c r="C53" s="7">
         <v>1</v>
       </c>
       <c r="D53" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="F53" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="G53" s="7">
+        <v>1</v>
+      </c>
+      <c r="H53" s="7">
+        <v>1</v>
+      </c>
+      <c r="J53" s="6">
+        <f t="shared" si="16"/>
+        <v>1.3247863247863249E-2</v>
+      </c>
+      <c r="K53" s="9">
+        <f t="shared" si="17"/>
+        <v>10.333333333333334</v>
+      </c>
+      <c r="L53" s="9">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="54" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="C54" s="7">
+        <v>1</v>
+      </c>
+      <c r="D54" s="7" t="s">
         <v>20</v>
-      </c>
-      <c r="F53" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="G53" s="7">
-        <v>4</v>
-      </c>
-      <c r="H53" s="7">
-        <v>1</v>
-      </c>
-      <c r="J53" s="6">
-        <f t="shared" si="14"/>
-        <v>5.8012820512820515E-2</v>
-      </c>
-      <c r="K53" s="9">
-        <f t="shared" si="15"/>
-        <v>45.25</v>
-      </c>
-      <c r="L53" s="9">
-        <v>543</v>
-      </c>
-    </row>
-    <row r="54" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="C54" s="7">
-        <v>1</v>
-      </c>
-      <c r="D54" s="7" t="s">
-        <v>16</v>
       </c>
       <c r="F54" s="4" t="s">
         <v>18</v>
@@ -2142,37 +2148,65 @@
         <v>1</v>
       </c>
       <c r="J54" s="6">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>5.8012820512820515E-2</v>
       </c>
       <c r="K54" s="9">
-        <f t="shared" si="15"/>
+        <f t="shared" si="17"/>
         <v>45.25</v>
       </c>
       <c r="L54" s="9">
         <v>543</v>
       </c>
     </row>
-    <row r="56" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="C56" s="1">
-        <f>SUM(C49:C55)</f>
+    <row r="55" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="C55" s="7">
+        <v>1</v>
+      </c>
+      <c r="D55" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="F55" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="G55" s="7">
+        <v>4</v>
+      </c>
+      <c r="H55" s="7">
+        <v>1</v>
+      </c>
+      <c r="J55" s="6">
+        <f t="shared" si="16"/>
+        <v>5.8012820512820515E-2</v>
+      </c>
+      <c r="K55" s="9">
+        <f t="shared" si="17"/>
+        <v>45.25</v>
+      </c>
+      <c r="L55" s="9">
+        <v>543</v>
+      </c>
+    </row>
+    <row r="57" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="C57" s="1">
+        <f>SUM(C50:C56)</f>
         <v>6</v>
       </c>
-      <c r="D56" s="1"/>
-      <c r="F56" s="1"/>
-      <c r="G56" s="1"/>
-      <c r="H56" s="1"/>
-      <c r="I56" s="1"/>
-      <c r="J56" s="3">
-        <f>SUM(J49:J55)</f>
+      <c r="D57" s="1"/>
+      <c r="F57" s="1"/>
+      <c r="G57" s="1"/>
+      <c r="H57" s="1"/>
+      <c r="I57" s="1"/>
+      <c r="J57" s="3">
+        <f>SUM(J50:J56)</f>
         <v>0.16901709401709403</v>
       </c>
-      <c r="K56" s="2">
-        <f>SUM(K49:K55)</f>
+      <c r="K57" s="2">
+        <f>SUM(K50:K56)</f>
         <v>131.83333333333334</v>
       </c>
-      <c r="L56" s="2">
-        <f>SUM(L49:L55)</f>
+      <c r="L57" s="2">
+        <f>SUM(L50:L56)</f>
         <v>1582</v>
       </c>
     </row>

</xml_diff>